<commit_message>
Aggiornamento Variable e AnalysisUnit
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/22_Inst_Analysis_Unit_BE.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/22_Inst_Analysis_Unit_BE.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giustino.matteo\Desktop\Progetto Early Warning\Materials_For_3DayTraining\Git\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="16635" yWindow="0" windowWidth="18315" windowHeight="7380" activeTab="1"/>
   </bookViews>
@@ -21,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +50,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="240">
   <si>
     <t>Analysis_Unit</t>
   </si>
@@ -268,16 +273,539 @@
   </si>
   <si>
     <t>COUNTERPARTY_BIB_IND_56</t>
+  </si>
+  <si>
+    <t>BE_IND_58</t>
+  </si>
+  <si>
+    <t>BE_IND_59</t>
+  </si>
+  <si>
+    <t>BE_IND_60</t>
+  </si>
+  <si>
+    <t>BE_IND_61</t>
+  </si>
+  <si>
+    <t>BE_IND_62</t>
+  </si>
+  <si>
+    <t>BE_IND_63</t>
+  </si>
+  <si>
+    <t>BE_IND_64</t>
+  </si>
+  <si>
+    <t>BE_IND_66</t>
+  </si>
+  <si>
+    <t>BE_IND_68</t>
+  </si>
+  <si>
+    <t>BE_IND_69</t>
+  </si>
+  <si>
+    <t>BE_IND_70</t>
+  </si>
+  <si>
+    <t>BE_IND_71</t>
+  </si>
+  <si>
+    <t>BE_IND_74</t>
+  </si>
+  <si>
+    <t>BE_IND_75</t>
+  </si>
+  <si>
+    <t>BE_IND_76</t>
+  </si>
+  <si>
+    <t>BE_IND_77</t>
+  </si>
+  <si>
+    <t>BE_IND_78</t>
+  </si>
+  <si>
+    <t>BE_IND_79</t>
+  </si>
+  <si>
+    <t>BE_IND_80</t>
+  </si>
+  <si>
+    <t>BE_IND_81</t>
+  </si>
+  <si>
+    <t>BE_IND_82</t>
+  </si>
+  <si>
+    <t>BE_IND_83</t>
+  </si>
+  <si>
+    <t>BE_IND_84</t>
+  </si>
+  <si>
+    <t>BE_IND_85</t>
+  </si>
+  <si>
+    <t>BE_IND_86</t>
+  </si>
+  <si>
+    <t>BE_IND_87</t>
+  </si>
+  <si>
+    <t>BE_IND_88</t>
+  </si>
+  <si>
+    <t>BE_IND_89</t>
+  </si>
+  <si>
+    <t>BE_IND_90</t>
+  </si>
+  <si>
+    <t>BE_IND_92</t>
+  </si>
+  <si>
+    <t>BE_IND_94</t>
+  </si>
+  <si>
+    <t>BE_IND_95</t>
+  </si>
+  <si>
+    <t>BE_IND_96</t>
+  </si>
+  <si>
+    <t>BE_IND_97</t>
+  </si>
+  <si>
+    <t>BE_IND_98</t>
+  </si>
+  <si>
+    <t>BE_IND_99</t>
+  </si>
+  <si>
+    <t>BE_IND_100</t>
+  </si>
+  <si>
+    <t>BE_IND_102</t>
+  </si>
+  <si>
+    <t>BE_IND_103</t>
+  </si>
+  <si>
+    <t>BE_IND_104</t>
+  </si>
+  <si>
+    <t>BE_IND_105</t>
+  </si>
+  <si>
+    <t>BE_IND_106</t>
+  </si>
+  <si>
+    <t>BE_IND_107</t>
+  </si>
+  <si>
+    <t>BE_IND_108</t>
+  </si>
+  <si>
+    <t>BE_IND_109</t>
+  </si>
+  <si>
+    <t>BE_IND_110</t>
+  </si>
+  <si>
+    <t>BE_IND_111</t>
+  </si>
+  <si>
+    <t>BE_IND_112</t>
+  </si>
+  <si>
+    <t>BE_IND_113</t>
+  </si>
+  <si>
+    <t>BE_IND_114</t>
+  </si>
+  <si>
+    <t>BE_IND_115</t>
+  </si>
+  <si>
+    <t>BE_IND_116</t>
+  </si>
+  <si>
+    <t>BE_IND_118</t>
+  </si>
+  <si>
+    <t>BE_IND_120</t>
+  </si>
+  <si>
+    <t>BE_IND_124</t>
+  </si>
+  <si>
+    <t>BE_IND_125</t>
+  </si>
+  <si>
+    <t>BE_IND_126</t>
+  </si>
+  <si>
+    <t>BE_IND_127</t>
+  </si>
+  <si>
+    <t>BE_IND_128</t>
+  </si>
+  <si>
+    <t>BE_IND_129</t>
+  </si>
+  <si>
+    <t>BE_IND_130</t>
+  </si>
+  <si>
+    <t>BE_IND_131</t>
+  </si>
+  <si>
+    <t>BE_IND_132</t>
+  </si>
+  <si>
+    <t>BE_IND_133</t>
+  </si>
+  <si>
+    <t>BE_IND_172</t>
+  </si>
+  <si>
+    <t>BE_IND_173</t>
+  </si>
+  <si>
+    <t>BE_IND_174</t>
+  </si>
+  <si>
+    <t>BE_IND_175</t>
+  </si>
+  <si>
+    <t>BE_IND_180</t>
+  </si>
+  <si>
+    <t>BE_IND_181</t>
+  </si>
+  <si>
+    <t>BE_IND_182</t>
+  </si>
+  <si>
+    <t>BE_IND_183</t>
+  </si>
+  <si>
+    <t>BE_IND_186</t>
+  </si>
+  <si>
+    <t>BE_IND_187</t>
+  </si>
+  <si>
+    <t>BE_IND_188</t>
+  </si>
+  <si>
+    <t>BE_IND_193</t>
+  </si>
+  <si>
+    <t>BE_IND_197</t>
+  </si>
+  <si>
+    <t>BE_IND_201</t>
+  </si>
+  <si>
+    <t>BE_IND_205</t>
+  </si>
+  <si>
+    <t>BE_IND_211</t>
+  </si>
+  <si>
+    <t>BE_IND_212</t>
+  </si>
+  <si>
+    <t>BE_IND_213</t>
+  </si>
+  <si>
+    <t>BE_IND_215</t>
+  </si>
+  <si>
+    <t>BE_IND_216</t>
+  </si>
+  <si>
+    <t>BE_IND_217</t>
+  </si>
+  <si>
+    <t>BE_IND_218</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_58</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_59</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_60</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_61</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_62</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_63</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_64</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_66</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_68</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_69</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_70</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_71</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_74</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_75</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_76</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_77</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_78</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_79</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_80</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_81</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_82</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_83</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_84</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_85</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_86</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_87</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_88</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_89</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_90</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_92</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_94</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_95</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_96</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_97</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_98</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_99</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_100</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_102</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_103</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_104</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_105</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_106</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_107</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_108</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_109</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_110</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_111</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_112</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_113</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_114</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_115</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_116</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_118</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_120</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_124</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_125</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_126</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_127</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_128</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_129</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_130</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_131</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_132</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_133</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_172</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_173</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_174</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_175</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_180</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_181</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_182</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_183</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_186</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_187</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_188</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_193</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_197</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_201</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_205</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_211</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_212</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_213</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_215</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_216</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_217</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIB_IND_218</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -299,6 +827,13 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -323,19 +858,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Variable" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -989,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1096,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,6 +1982,1468 @@
       </c>
       <c r="F20" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" t="s">
+        <v>180</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
+        <v>183</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" t="s">
+        <v>185</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>188</v>
+      </c>
+      <c r="C55" t="s">
+        <v>188</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+      <c r="F55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E56" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>193</v>
+      </c>
+      <c r="C60" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" t="s">
+        <v>194</v>
+      </c>
+      <c r="E61" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>195</v>
+      </c>
+      <c r="C62" t="s">
+        <v>195</v>
+      </c>
+      <c r="E62" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" t="s">
+        <v>196</v>
+      </c>
+      <c r="E63" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" t="s">
+        <v>197</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+      <c r="E65" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" t="s">
+        <v>200</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>201</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>202</v>
+      </c>
+      <c r="C69" t="s">
+        <v>202</v>
+      </c>
+      <c r="E69" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" t="s">
+        <v>203</v>
+      </c>
+      <c r="E70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>204</v>
+      </c>
+      <c r="C71" t="s">
+        <v>204</v>
+      </c>
+      <c r="E71" t="s">
+        <v>33</v>
+      </c>
+      <c r="F71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" t="s">
+        <v>205</v>
+      </c>
+      <c r="E72" t="s">
+        <v>33</v>
+      </c>
+      <c r="F72" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>206</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+      <c r="F73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" t="s">
+        <v>33</v>
+      </c>
+      <c r="F74" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>208</v>
+      </c>
+      <c r="C75" t="s">
+        <v>208</v>
+      </c>
+      <c r="E75" t="s">
+        <v>33</v>
+      </c>
+      <c r="F75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" t="s">
+        <v>209</v>
+      </c>
+      <c r="E76" t="s">
+        <v>33</v>
+      </c>
+      <c r="F76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" t="s">
+        <v>210</v>
+      </c>
+      <c r="E77" t="s">
+        <v>33</v>
+      </c>
+      <c r="F77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" t="s">
+        <v>211</v>
+      </c>
+      <c r="E78" t="s">
+        <v>33</v>
+      </c>
+      <c r="F78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" t="s">
+        <v>212</v>
+      </c>
+      <c r="E79" t="s">
+        <v>33</v>
+      </c>
+      <c r="F79" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" t="s">
+        <v>213</v>
+      </c>
+      <c r="C80" t="s">
+        <v>213</v>
+      </c>
+      <c r="E80" t="s">
+        <v>33</v>
+      </c>
+      <c r="F80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>214</v>
+      </c>
+      <c r="C81" t="s">
+        <v>214</v>
+      </c>
+      <c r="E81" t="s">
+        <v>33</v>
+      </c>
+      <c r="F81" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" t="s">
+        <v>215</v>
+      </c>
+      <c r="E82" t="s">
+        <v>33</v>
+      </c>
+      <c r="F82" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" t="s">
+        <v>33</v>
+      </c>
+      <c r="F83" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>217</v>
+      </c>
+      <c r="C84" t="s">
+        <v>217</v>
+      </c>
+      <c r="E84" t="s">
+        <v>33</v>
+      </c>
+      <c r="F84" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85" t="s">
+        <v>218</v>
+      </c>
+      <c r="E85" t="s">
+        <v>33</v>
+      </c>
+      <c r="F85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>219</v>
+      </c>
+      <c r="C86" t="s">
+        <v>219</v>
+      </c>
+      <c r="E86" t="s">
+        <v>33</v>
+      </c>
+      <c r="F86" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
+        <v>220</v>
+      </c>
+      <c r="C87" t="s">
+        <v>220</v>
+      </c>
+      <c r="E87" t="s">
+        <v>33</v>
+      </c>
+      <c r="F87" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>221</v>
+      </c>
+      <c r="C88" t="s">
+        <v>221</v>
+      </c>
+      <c r="E88" t="s">
+        <v>33</v>
+      </c>
+      <c r="F88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>222</v>
+      </c>
+      <c r="C89" t="s">
+        <v>222</v>
+      </c>
+      <c r="E89" t="s">
+        <v>33</v>
+      </c>
+      <c r="F89" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" t="s">
+        <v>223</v>
+      </c>
+      <c r="C90" t="s">
+        <v>223</v>
+      </c>
+      <c r="E90" t="s">
+        <v>33</v>
+      </c>
+      <c r="F90" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" t="s">
+        <v>224</v>
+      </c>
+      <c r="C91" t="s">
+        <v>224</v>
+      </c>
+      <c r="E91" t="s">
+        <v>33</v>
+      </c>
+      <c r="F91" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" t="s">
+        <v>225</v>
+      </c>
+      <c r="E92" t="s">
+        <v>33</v>
+      </c>
+      <c r="F92" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" t="s">
+        <v>226</v>
+      </c>
+      <c r="C93" t="s">
+        <v>226</v>
+      </c>
+      <c r="E93" t="s">
+        <v>33</v>
+      </c>
+      <c r="F93" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" t="s">
+        <v>227</v>
+      </c>
+      <c r="C94" t="s">
+        <v>227</v>
+      </c>
+      <c r="E94" t="s">
+        <v>33</v>
+      </c>
+      <c r="F94" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B95" t="s">
+        <v>228</v>
+      </c>
+      <c r="C95" t="s">
+        <v>228</v>
+      </c>
+      <c r="E95" t="s">
+        <v>33</v>
+      </c>
+      <c r="F95" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" t="s">
+        <v>229</v>
+      </c>
+      <c r="E96" t="s">
+        <v>33</v>
+      </c>
+      <c r="F96" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B97" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" t="s">
+        <v>230</v>
+      </c>
+      <c r="E97" t="s">
+        <v>33</v>
+      </c>
+      <c r="F97" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B98" t="s">
+        <v>231</v>
+      </c>
+      <c r="C98" t="s">
+        <v>231</v>
+      </c>
+      <c r="E98" t="s">
+        <v>33</v>
+      </c>
+      <c r="F98" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+      <c r="C99" t="s">
+        <v>232</v>
+      </c>
+      <c r="E99" t="s">
+        <v>33</v>
+      </c>
+      <c r="F99" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B100" t="s">
+        <v>233</v>
+      </c>
+      <c r="C100" t="s">
+        <v>233</v>
+      </c>
+      <c r="E100" t="s">
+        <v>33</v>
+      </c>
+      <c r="F100" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" t="s">
+        <v>234</v>
+      </c>
+      <c r="E101" t="s">
+        <v>33</v>
+      </c>
+      <c r="F101" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>235</v>
+      </c>
+      <c r="C102" t="s">
+        <v>235</v>
+      </c>
+      <c r="E102" t="s">
+        <v>33</v>
+      </c>
+      <c r="F102" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s">
+        <v>236</v>
+      </c>
+      <c r="C103" t="s">
+        <v>236</v>
+      </c>
+      <c r="E103" t="s">
+        <v>33</v>
+      </c>
+      <c r="F103" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s">
+        <v>237</v>
+      </c>
+      <c r="C104" t="s">
+        <v>237</v>
+      </c>
+      <c r="E104" t="s">
+        <v>33</v>
+      </c>
+      <c r="F104" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s">
+        <v>238</v>
+      </c>
+      <c r="C105" t="s">
+        <v>238</v>
+      </c>
+      <c r="E105" t="s">
+        <v>33</v>
+      </c>
+      <c r="F105" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" t="s">
+        <v>239</v>
+      </c>
+      <c r="C106" t="s">
+        <v>239</v>
+      </c>
+      <c r="E106" t="s">
+        <v>33</v>
+      </c>
+      <c r="F106" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>